<commit_message>
Oprava reportu a komentaru
</commit_message>
<xml_diff>
--- a/results/mereni.xlsx
+++ b/results/mereni.xlsx
@@ -435,12 +435,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
@@ -450,15 +444,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -466,12 +454,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -485,6 +467,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="normální" xfId="0" builtinId="0"/>
@@ -518,8 +518,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.38761261261261259"/>
-          <c:y val="2.1621621621621623E-2"/>
+          <c:x val="0.38761261261261271"/>
+          <c:y val="2.162162162162163E-2"/>
         </c:manualLayout>
       </c:layout>
     </c:title>
@@ -715,12 +715,12 @@
           </c:val>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="70793472"/>
-        <c:axId val="70824704"/>
+        <c:axId val="83250560"/>
+        <c:axId val="83273600"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="70793472"/>
+        <c:axId val="83250560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -744,14 +744,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70824704"/>
+        <c:crossAx val="83273600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="70824704"/>
+        <c:axId val="83273600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -777,7 +777,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70793472"/>
+        <c:crossAx val="83250560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -790,7 +790,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000007" r="0.70000000000000007" t="0.78740157499999996" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1015,12 +1015,12 @@
           </c:val>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="101184256"/>
-        <c:axId val="114349184"/>
+        <c:axId val="84037632"/>
+        <c:axId val="84039552"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="101184256"/>
+        <c:axId val="84037632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1044,14 +1044,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114349184"/>
+        <c:crossAx val="84039552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="114349184"/>
+        <c:axId val="84039552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1077,7 +1077,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101184256"/>
+        <c:crossAx val="84037632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1090,7 +1090,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000007" r="0.70000000000000007" t="0.78740157499999996" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1188,69 +1188,8 @@
           </c:val>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="2"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:v>DFS</c:v>
-          </c:tx>
-          <c:val>
-            <c:numRef>
-              <c:f>List1!$X$4:$X$18</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
-                <c:pt idx="0">
-                  <c:v>1125</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>836</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>318</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>469</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>475</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
           <c:tx>
             <c:v>Heuristika</c:v>
           </c:tx>
@@ -1310,12 +1249,12 @@
           </c:val>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="117276032"/>
-        <c:axId val="117828224"/>
+        <c:axId val="84082688"/>
+        <c:axId val="84084608"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="117276032"/>
+        <c:axId val="84082688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1344,14 +1283,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="117828224"/>
+        <c:crossAx val="84084608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="117828224"/>
+        <c:axId val="84084608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1377,7 +1316,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="117276032"/>
+        <c:crossAx val="84082688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1390,7 +1329,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000007" r="0.70000000000000007" t="0.78740157499999996" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1778,7 +1717,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Y38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
       <selection activeCell="A24" sqref="A24:C38"/>
     </sheetView>
   </sheetViews>
@@ -1799,68 +1738,68 @@
       </c>
     </row>
     <row r="2" spans="1:25">
-      <c r="A2" s="36"/>
-      <c r="B2" s="19" t="s">
+      <c r="A2" s="30"/>
+      <c r="B2" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="23" t="s">
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="28" t="s">
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="28"/>
-      <c r="J2" s="29"/>
-      <c r="L2" s="8" t="s">
+      <c r="I2" s="36"/>
+      <c r="J2" s="37"/>
+      <c r="L2" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
       <c r="P2" s="1"/>
-      <c r="Q2" s="9" t="s">
+      <c r="Q2" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="R2" s="9"/>
-      <c r="S2" s="9"/>
-      <c r="T2" s="9"/>
+      <c r="R2" s="39"/>
+      <c r="S2" s="39"/>
+      <c r="T2" s="39"/>
       <c r="V2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:25">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="F3" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="24" t="s">
+      <c r="G3" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="30" t="s">
+      <c r="H3" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="30" t="s">
+      <c r="I3" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="31" t="s">
+      <c r="J3" s="25" t="s">
         <v>22</v>
       </c>
       <c r="L3" s="4"/>
@@ -1895,34 +1834,34 @@
       </c>
     </row>
     <row r="4" spans="1:25">
-      <c r="A4" s="38">
+      <c r="A4" s="32">
         <v>11</v>
       </c>
-      <c r="B4" s="21">
+      <c r="B4" s="18">
         <v>10</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="18">
         <v>8992</v>
       </c>
-      <c r="D4" s="21">
+      <c r="D4" s="18">
         <v>106125</v>
       </c>
-      <c r="E4" s="25">
+      <c r="E4" s="21">
         <v>1125</v>
       </c>
-      <c r="F4" s="25">
+      <c r="F4" s="21">
         <v>4870</v>
       </c>
-      <c r="G4" s="25">
+      <c r="G4" s="21">
         <v>57563</v>
       </c>
-      <c r="H4" s="32">
+      <c r="H4" s="26">
         <v>19</v>
       </c>
-      <c r="I4" s="32">
+      <c r="I4" s="26">
         <v>295</v>
       </c>
-      <c r="J4" s="33">
+      <c r="J4" s="27">
         <v>1061</v>
       </c>
       <c r="L4">
@@ -1963,34 +1902,34 @@
       </c>
     </row>
     <row r="5" spans="1:25">
-      <c r="A5" s="38">
+      <c r="A5" s="32">
         <v>12</v>
       </c>
-      <c r="B5" s="21">
+      <c r="B5" s="18">
         <v>8</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="18">
         <v>8084</v>
       </c>
-      <c r="D5" s="21">
+      <c r="D5" s="18">
         <v>80165</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="21">
         <v>836</v>
       </c>
-      <c r="F5" s="25">
+      <c r="F5" s="21">
         <v>5521</v>
       </c>
-      <c r="G5" s="25">
+      <c r="G5" s="21">
         <v>68987</v>
       </c>
-      <c r="H5" s="32">
+      <c r="H5" s="26">
         <v>9</v>
       </c>
-      <c r="I5" s="32">
+      <c r="I5" s="26">
         <v>268</v>
       </c>
-      <c r="J5" s="33">
+      <c r="J5" s="27">
         <v>530</v>
       </c>
       <c r="L5">
@@ -2031,34 +1970,34 @@
       </c>
     </row>
     <row r="6" spans="1:25">
-      <c r="A6" s="38">
+      <c r="A6" s="32">
         <v>13</v>
       </c>
-      <c r="B6" s="21">
+      <c r="B6" s="18">
         <v>8</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6" s="18">
         <v>7914</v>
       </c>
-      <c r="D6" s="21">
+      <c r="D6" s="18">
         <v>78721</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="21">
         <v>318</v>
       </c>
-      <c r="F6" s="25">
+      <c r="F6" s="21">
         <v>742</v>
       </c>
-      <c r="G6" s="25">
+      <c r="G6" s="21">
         <v>2400</v>
       </c>
-      <c r="H6" s="32">
+      <c r="H6" s="26">
         <v>23</v>
       </c>
-      <c r="I6" s="32">
+      <c r="I6" s="26">
         <v>35</v>
       </c>
-      <c r="J6" s="33">
+      <c r="J6" s="27">
         <v>16</v>
       </c>
       <c r="L6">
@@ -2099,34 +2038,34 @@
       </c>
     </row>
     <row r="7" spans="1:25">
-      <c r="A7" s="38">
+      <c r="A7" s="32">
         <v>14</v>
       </c>
-      <c r="B7" s="21">
+      <c r="B7" s="18">
         <v>3</v>
       </c>
-      <c r="C7" s="21">
+      <c r="C7" s="18">
         <v>170</v>
       </c>
-      <c r="D7" s="21">
+      <c r="D7" s="18">
         <v>117</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="21">
         <v>5</v>
       </c>
-      <c r="F7" s="25">
+      <c r="F7" s="21">
         <v>8953</v>
       </c>
-      <c r="G7" s="25">
+      <c r="G7" s="21">
         <v>109536</v>
       </c>
-      <c r="H7" s="32">
+      <c r="H7" s="26">
         <v>11</v>
       </c>
-      <c r="I7" s="32">
+      <c r="I7" s="26">
         <v>597</v>
       </c>
-      <c r="J7" s="33">
+      <c r="J7" s="27">
         <v>2340</v>
       </c>
       <c r="L7">
@@ -2167,34 +2106,34 @@
       </c>
     </row>
     <row r="8" spans="1:25">
-      <c r="A8" s="38">
+      <c r="A8" s="32">
         <v>21</v>
       </c>
-      <c r="B8" s="21">
+      <c r="B8" s="18">
         <v>16</v>
       </c>
-      <c r="C8" s="21">
+      <c r="C8" s="18">
         <v>49350</v>
       </c>
-      <c r="D8" s="21">
+      <c r="D8" s="18">
         <v>3499577</v>
       </c>
-      <c r="E8" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="G8" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="H8" s="32">
+      <c r="E8" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="26">
         <v>42</v>
       </c>
-      <c r="I8" s="32">
+      <c r="I8" s="26">
         <v>586</v>
       </c>
-      <c r="J8" s="33">
+      <c r="J8" s="27">
         <v>2402</v>
       </c>
       <c r="L8">
@@ -2235,34 +2174,34 @@
       </c>
     </row>
     <row r="9" spans="1:25">
-      <c r="A9" s="38">
+      <c r="A9" s="32">
         <v>22</v>
       </c>
-      <c r="B9" s="21">
+      <c r="B9" s="18">
         <v>12</v>
       </c>
-      <c r="C9" s="21">
+      <c r="C9" s="18">
         <v>41669</v>
       </c>
-      <c r="D9" s="21">
+      <c r="D9" s="18">
         <v>2540323</v>
       </c>
-      <c r="E9" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="G9" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="H9" s="32">
+      <c r="E9" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" s="26">
         <v>52</v>
       </c>
-      <c r="I9" s="32">
+      <c r="I9" s="26">
         <v>618</v>
       </c>
-      <c r="J9" s="33">
+      <c r="J9" s="27">
         <v>6755</v>
       </c>
       <c r="L9">
@@ -2303,34 +2242,34 @@
       </c>
     </row>
     <row r="10" spans="1:25">
-      <c r="A10" s="38">
+      <c r="A10" s="32">
         <v>23</v>
       </c>
-      <c r="B10" s="21">
+      <c r="B10" s="18">
         <v>11</v>
       </c>
-      <c r="C10" s="21">
+      <c r="C10" s="18">
         <v>35750</v>
       </c>
-      <c r="D10" s="21">
+      <c r="D10" s="18">
         <v>1861169</v>
       </c>
-      <c r="E10" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="G10" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="H10" s="32">
+      <c r="E10" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" s="26">
         <v>38</v>
       </c>
-      <c r="I10" s="32">
+      <c r="I10" s="26">
         <v>827</v>
       </c>
-      <c r="J10" s="33">
+      <c r="J10" s="27">
         <v>12340</v>
       </c>
       <c r="L10">
@@ -2371,34 +2310,34 @@
       </c>
     </row>
     <row r="11" spans="1:25">
-      <c r="A11" s="38">
+      <c r="A11" s="32">
         <v>24</v>
       </c>
-      <c r="B11" s="21">
+      <c r="B11" s="18">
         <v>5</v>
       </c>
-      <c r="C11" s="21">
+      <c r="C11" s="18">
         <v>872</v>
       </c>
-      <c r="D11" s="21">
+      <c r="D11" s="18">
         <v>1513</v>
       </c>
-      <c r="E11" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="F11" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="G11" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="H11" s="32">
+      <c r="E11" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="H11" s="26">
         <v>18</v>
       </c>
-      <c r="I11" s="32">
+      <c r="I11" s="26">
         <v>1604</v>
       </c>
-      <c r="J11" s="33">
+      <c r="J11" s="27">
         <v>12090</v>
       </c>
       <c r="L11">
@@ -2439,34 +2378,34 @@
       </c>
     </row>
     <row r="12" spans="1:25">
-      <c r="A12" s="38">
+      <c r="A12" s="32">
         <v>25</v>
       </c>
-      <c r="B12" s="21">
+      <c r="B12" s="18">
         <v>7</v>
       </c>
-      <c r="C12" s="21">
+      <c r="C12" s="18">
         <v>6324</v>
       </c>
-      <c r="D12" s="21">
+      <c r="D12" s="18">
         <v>58427</v>
       </c>
-      <c r="E12" s="25">
+      <c r="E12" s="21">
         <v>4692</v>
       </c>
-      <c r="F12" s="25">
+      <c r="F12" s="21">
         <v>4848</v>
       </c>
-      <c r="G12" s="25">
+      <c r="G12" s="21">
         <v>241919</v>
       </c>
-      <c r="H12" s="32">
+      <c r="H12" s="26">
         <v>37</v>
       </c>
-      <c r="I12" s="32">
+      <c r="I12" s="26">
         <v>839</v>
       </c>
-      <c r="J12" s="33">
+      <c r="J12" s="27">
         <v>4929</v>
       </c>
       <c r="L12">
@@ -2507,34 +2446,34 @@
       </c>
     </row>
     <row r="13" spans="1:25">
-      <c r="A13" s="38">
+      <c r="A13" s="32">
         <v>31</v>
       </c>
-      <c r="B13" s="21">
+      <c r="B13" s="18">
         <v>14</v>
       </c>
-      <c r="C13" s="21">
+      <c r="C13" s="18">
         <v>59200</v>
       </c>
-      <c r="D13" s="21">
+      <c r="D13" s="18">
         <v>4975088</v>
       </c>
-      <c r="E13" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="F13" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="G13" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="H13" s="32">
+      <c r="E13" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="H13" s="26">
         <v>20</v>
       </c>
-      <c r="I13" s="32">
+      <c r="I13" s="26">
         <v>884</v>
       </c>
-      <c r="J13" s="33">
+      <c r="J13" s="27">
         <v>10889</v>
       </c>
       <c r="L13">
@@ -2575,34 +2514,34 @@
       </c>
     </row>
     <row r="14" spans="1:25">
-      <c r="A14" s="38">
+      <c r="A14" s="32">
         <v>32</v>
       </c>
-      <c r="B14" s="21">
+      <c r="B14" s="18">
         <v>12</v>
       </c>
-      <c r="C14" s="21">
+      <c r="C14" s="18">
         <v>58772</v>
       </c>
-      <c r="D14" s="21">
+      <c r="D14" s="18">
         <v>4781442</v>
       </c>
-      <c r="E14" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="F14" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="G14" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="H14" s="32">
+      <c r="E14" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="H14" s="26">
         <v>30</v>
       </c>
-      <c r="I14" s="32">
+      <c r="I14" s="26">
         <v>423</v>
       </c>
-      <c r="J14" s="33">
+      <c r="J14" s="27">
         <v>3713</v>
       </c>
       <c r="L14">
@@ -2643,34 +2582,34 @@
       </c>
     </row>
     <row r="15" spans="1:25">
-      <c r="A15" s="38">
+      <c r="A15" s="32">
         <v>33</v>
       </c>
-      <c r="B15" s="21">
+      <c r="B15" s="18">
         <v>10</v>
       </c>
-      <c r="C15" s="21">
+      <c r="C15" s="18">
         <v>40908</v>
       </c>
-      <c r="D15" s="21">
+      <c r="D15" s="18">
         <v>2240414</v>
       </c>
-      <c r="E15" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="G15" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="H15" s="32">
+      <c r="E15" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="H15" s="26">
         <v>23</v>
       </c>
-      <c r="I15" s="32">
+      <c r="I15" s="26">
         <v>1377</v>
       </c>
-      <c r="J15" s="33">
+      <c r="J15" s="27">
         <v>14664</v>
       </c>
       <c r="L15">
@@ -2711,34 +2650,34 @@
       </c>
     </row>
     <row r="16" spans="1:25">
-      <c r="A16" s="38">
+      <c r="A16" s="32">
         <v>34</v>
       </c>
-      <c r="B16" s="21">
+      <c r="B16" s="18">
         <v>5</v>
       </c>
-      <c r="C16" s="21">
+      <c r="C16" s="18">
         <v>1461</v>
       </c>
-      <c r="D16" s="21">
+      <c r="D16" s="18">
         <v>4555</v>
       </c>
-      <c r="E16" s="25">
+      <c r="E16" s="21">
         <v>475</v>
       </c>
-      <c r="F16" s="25">
+      <c r="F16" s="21">
         <v>476</v>
       </c>
-      <c r="G16" s="25">
+      <c r="G16" s="21">
         <v>1758</v>
       </c>
-      <c r="H16" s="32">
+      <c r="H16" s="26">
         <v>6</v>
       </c>
-      <c r="I16" s="32">
+      <c r="I16" s="26">
         <v>264</v>
       </c>
-      <c r="J16" s="33">
+      <c r="J16" s="27">
         <v>359</v>
       </c>
       <c r="L16">
@@ -2779,34 +2718,34 @@
       </c>
     </row>
     <row r="17" spans="1:25">
-      <c r="A17" s="38">
+      <c r="A17" s="32">
         <v>35</v>
       </c>
-      <c r="B17" s="21">
+      <c r="B17" s="18">
         <v>7</v>
       </c>
-      <c r="C17" s="21">
+      <c r="C17" s="18">
         <v>9155</v>
       </c>
-      <c r="D17" s="21">
+      <c r="D17" s="18">
         <v>122913</v>
       </c>
-      <c r="E17" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="F17" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="G17" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="H17" s="32">
+      <c r="E17" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="G17" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="H17" s="26">
         <v>20</v>
       </c>
-      <c r="I17" s="32">
+      <c r="I17" s="26">
         <v>100</v>
       </c>
-      <c r="J17" s="33">
+      <c r="J17" s="27">
         <v>156</v>
       </c>
       <c r="L17">
@@ -2847,34 +2786,34 @@
       </c>
     </row>
     <row r="18" spans="1:25">
-      <c r="A18" s="39">
+      <c r="A18" s="33">
         <v>36</v>
       </c>
-      <c r="B18" s="22">
+      <c r="B18" s="19">
         <v>9</v>
       </c>
-      <c r="C18" s="22">
+      <c r="C18" s="19">
         <v>27773</v>
       </c>
-      <c r="D18" s="22">
+      <c r="D18" s="19">
         <v>1039404</v>
       </c>
-      <c r="E18" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="F18" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G18" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="H18" s="34">
+      <c r="E18" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="G18" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="H18" s="28">
         <v>24</v>
       </c>
-      <c r="I18" s="34">
+      <c r="I18" s="28">
         <v>279</v>
       </c>
-      <c r="J18" s="35">
+      <c r="J18" s="29">
         <v>717</v>
       </c>
       <c r="L18" s="4">
@@ -2915,58 +2854,58 @@
       </c>
     </row>
     <row r="19" spans="1:25">
-      <c r="A19" s="14"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="16">
+      <c r="A19" s="12"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="14">
         <f>SUM(C4:C18)</f>
         <v>356394</v>
       </c>
-      <c r="D19" s="16">
+      <c r="D19" s="14">
         <f>SUM(D4:D18)/1000</f>
         <v>21389.953000000001</v>
       </c>
-      <c r="E19" s="17"/>
-      <c r="F19" s="16">
+      <c r="E19" s="15"/>
+      <c r="F19" s="14">
         <f>SUM(F4:F18)</f>
         <v>25410</v>
       </c>
-      <c r="G19" s="16">
+      <c r="G19" s="14">
         <f>SUM(G4:G18)/1000</f>
         <v>482.16300000000001</v>
       </c>
-      <c r="H19" s="17"/>
-      <c r="I19" s="16">
+      <c r="H19" s="15"/>
+      <c r="I19" s="14">
         <f>SUM(I4:I18)</f>
         <v>8996</v>
       </c>
-      <c r="J19" s="18">
+      <c r="J19" s="16">
         <f>SUM(J4:J18)/1000</f>
         <v>72.960999999999999</v>
       </c>
     </row>
     <row r="20" spans="1:25">
-      <c r="A20" s="10"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="12" t="s">
+      <c r="A20" s="8"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="12">
+      <c r="D20" s="10">
         <f>C19/D19</f>
         <v>16.661747690609698</v>
       </c>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12" t="s">
+      <c r="E20" s="10"/>
+      <c r="F20" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="G20" s="12">
+      <c r="G20" s="10">
         <f>F19/G19</f>
         <v>52.700020532475534</v>
       </c>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12" t="s">
+      <c r="H20" s="10"/>
+      <c r="I20" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="J20" s="13">
+      <c r="J20" s="11">
         <f>I19/J19</f>
         <v>123.29874864653719</v>
       </c>

</xml_diff>